<commit_message>
Set the Luddite events loops to much more realistic probabilities
</commit_message>
<xml_diff>
--- a/MTTH Probability Calculator.xlsx
+++ b/MTTH Probability Calculator.xlsx
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23775018-7EFC-4F53-B33C-17EB9D8D2067}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -403,14 +403,15 @@
     <col min="4" max="4" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.75">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -424,20 +425,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C6">
         <f>1-(0.5)^(F6/E6)</f>
-        <v>0.20629947401590021</v>
+        <v>1.148597964710385E-2</v>
       </c>
       <c r="D6">
         <f>F6*(1-0.5^(1/E6))</f>
-        <v>0.2301616121116945</v>
+        <v>1.1550228975311105E-2</v>
       </c>
       <c r="E6">
-        <v>90</v>
+        <f>60*30</f>
+        <v>1800</v>
       </c>
       <c r="F6">
         <v>30</v>
+      </c>
+      <c r="J6">
+        <f>1-(1-C6)^60</f>
+        <v>0.49999999999999856</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C7">
+        <f>1-(0.5)^(F7/E7)</f>
+        <v>1.6489893504895159E-3</v>
+      </c>
+      <c r="D7">
+        <f>F7*(1-0.5^(1/E7))</f>
+        <v>1.6489893504895159E-3</v>
+      </c>
+      <c r="E7">
+        <f>35*12</f>
+        <v>420</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C8">
+        <f>1-(0.5)^(F8/E8)</f>
+        <v>1.1545782619698519E-3</v>
+      </c>
+      <c r="D8">
+        <f>F8*(1-0.5^(1/E8))</f>
+        <v>1.1545782619698519E-3</v>
+      </c>
+      <c r="E8">
+        <v>600</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C9">
+        <f>1-(0.5)^(F9/E9)</f>
+        <v>4.5158396089583497E-2</v>
+      </c>
+      <c r="D9">
+        <f>F9*(1-0.5^(1/E9))</f>
+        <v>4.6103208967709364E-2</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C10">
+        <f>1-(0.5)^(F10/E10)</f>
+        <v>3.7776163105854854E-2</v>
+      </c>
+      <c r="D10">
+        <f>F10*(1-0.5^(1/E10))</f>
+        <v>3.843412779424793E-2</v>
+      </c>
+      <c r="E10">
+        <v>180</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major work to get the Spiritualist Mission chain to something like 85% completion
</commit_message>
<xml_diff>
--- a/MTTH Probability Calculator.xlsx
+++ b/MTTH Probability Calculator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -390,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23775018-7EFC-4F53-B33C-17EB9D8D2067}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -511,6 +511,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C11">
+        <f>1-(0.5)^(F11/E11)</f>
+        <v>3.7776163105854854E-2</v>
+      </c>
+      <c r="D11">
+        <f>F11*(1-0.5^(1/E11))</f>
+        <v>3.8471128487425066E-2</v>
+      </c>
+      <c r="E11">
+        <v>360</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished adding HW localisations. Preparing release
</commit_message>
<xml_diff>
--- a/MTTH Probability Calculator.xlsx
+++ b/MTTH Probability Calculator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre\Documents\Paradox Interactive\Stellaris\mod\cc_events\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D50016-7BDA-47AD-AB3E-B93EC621E96E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6620" xr2:uid="{F48ED777-99F4-4B03-9516-3C10F224EC94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -390,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23775018-7EFC-4F53-B33C-17EB9D8D2067}">
-  <dimension ref="B2:J11"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -427,11 +428,11 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C6">
-        <f>1-(0.5)^(F6/E6)</f>
+        <f t="shared" ref="C6:C12" si="0">1-(0.5)^(F6/E6)</f>
         <v>1.148597964710385E-2</v>
       </c>
       <c r="D6">
-        <f>F6*(1-0.5^(1/E6))</f>
+        <f t="shared" ref="D6:D12" si="1">F6*(1-0.5^(1/E6))</f>
         <v>1.1550228975311105E-2</v>
       </c>
       <c r="E6">
@@ -448,11 +449,11 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C7">
-        <f>1-(0.5)^(F7/E7)</f>
+        <f t="shared" si="0"/>
         <v>1.6489893504895159E-3</v>
       </c>
       <c r="D7">
-        <f>F7*(1-0.5^(1/E7))</f>
+        <f t="shared" si="1"/>
         <v>1.6489893504895159E-3</v>
       </c>
       <c r="E7">
@@ -465,11 +466,11 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C8">
-        <f>1-(0.5)^(F8/E8)</f>
+        <f t="shared" si="0"/>
         <v>1.1545782619698519E-3</v>
       </c>
       <c r="D8">
-        <f>F8*(1-0.5^(1/E8))</f>
+        <f t="shared" si="1"/>
         <v>1.1545782619698519E-3</v>
       </c>
       <c r="E8">
@@ -481,11 +482,11 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C9">
-        <f>1-(0.5)^(F9/E9)</f>
+        <f t="shared" si="0"/>
         <v>4.5158396089583497E-2</v>
       </c>
       <c r="D9">
-        <f>F9*(1-0.5^(1/E9))</f>
+        <f t="shared" si="1"/>
         <v>4.6103208967709364E-2</v>
       </c>
       <c r="E9">
@@ -497,11 +498,11 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C10">
-        <f>1-(0.5)^(F10/E10)</f>
+        <f t="shared" si="0"/>
         <v>3.7776163105854854E-2</v>
       </c>
       <c r="D10">
-        <f>F10*(1-0.5^(1/E10))</f>
+        <f t="shared" si="1"/>
         <v>3.843412779424793E-2</v>
       </c>
       <c r="E10">
@@ -513,17 +514,33 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.75">
       <c r="C11">
-        <f>1-(0.5)^(F11/E11)</f>
+        <f t="shared" si="0"/>
         <v>3.7776163105854854E-2</v>
       </c>
       <c r="D11">
-        <f>F11*(1-0.5^(1/E11))</f>
+        <f t="shared" si="1"/>
         <v>3.8471128487425066E-2</v>
       </c>
       <c r="E11">
         <v>360</v>
       </c>
       <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.5285247065568774E-2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1.539734068287224E-2</v>
+      </c>
+      <c r="E12">
+        <v>900</v>
+      </c>
+      <c r="F12">
         <v>20</v>
       </c>
     </row>

</xml_diff>